<commit_message>
Updated Project 3 with few final touches
</commit_message>
<xml_diff>
--- a/Udacity Preparing and Modelling Data/Project 3 Project Market Analysis Report for National Clothing Chain/Rubric and Screenshots/Rubric tracker.xlsx
+++ b/Udacity Preparing and Modelling Data/Project 3 Project Market Analysis Report for National Clothing Chain/Rubric and Screenshots/Rubric tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PowerBI\Power-BI\Udacity Preparing and Modelling Data\Project 3 Project Market Analysis Report for National Clothing Chain\Screenshots as per Rubric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PowerBI\Power-BI\Udacity Preparing and Modelling Data\Project 3 Project Market Analysis Report for National Clothing Chain\Rubric and Screenshots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B54A54C-AFA1-4E24-8F23-1B51CB5DE2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A925D17-93AC-4739-9F83-B870827628D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20617" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{0E040457-2FD3-47A4-81B4-7EB53601751D}"/>
+    <workbookView xWindow="22932" yWindow="1488" windowWidth="23256" windowHeight="13176" xr2:uid="{0E040457-2FD3-47A4-81B4-7EB53601751D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
   <si>
     <t>CRITERIA</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>11 Screenshot of cross-filtered scatterplot and heatmap</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -719,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD328A0-A231-4F37-9A45-D654683D7BC9}">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,48 +1034,72 @@
       <c r="B40" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="C40" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="C41" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="C42" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="C43" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="C44" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="C45" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C46" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C47" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
@@ -1080,131 +1107,167 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="B49" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="C49" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="43.5" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="29.25" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="C54" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="29.25" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="C55" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B56" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="C56" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B57" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C57" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B58" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B59" s="5"/>
     </row>
-    <row r="60" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B60" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B61" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B62" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B63" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B64" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C64" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B65" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="66" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C65" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B66" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B67" s="5"/>
     </row>
-    <row r="68" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B68" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B69" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:3" ht="33" x14ac:dyDescent="0.3">
       <c r="B70" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:3" ht="33" x14ac:dyDescent="0.3">
       <c r="B71" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B72" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="73" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C72" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="74" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C73" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B74" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="75" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C74" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B75" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="76" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C75" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B76" s="5" t="s">
         <v>71</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalised Project 3 Approved by Udacity
</commit_message>
<xml_diff>
--- a/Udacity Preparing and Modelling Data/Project 3 Project Market Analysis Report for National Clothing Chain/Rubric and Screenshots/Rubric tracker.xlsx
+++ b/Udacity Preparing and Modelling Data/Project 3 Project Market Analysis Report for National Clothing Chain/Rubric and Screenshots/Rubric tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PowerBI\Power-BI\Udacity Preparing and Modelling Data\Project 3 Project Market Analysis Report for National Clothing Chain\Rubric and Screenshots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A925D17-93AC-4739-9F83-B870827628D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35747FE-BD9A-4673-9CC2-63D251FAD0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="1488" windowWidth="23256" windowHeight="13176" xr2:uid="{0E040457-2FD3-47A4-81B4-7EB53601751D}"/>
   </bookViews>
@@ -258,9 +258,6 @@
     <t>3 Predicted Customer Income Bins DAX formula</t>
   </si>
   <si>
-    <t>4 Targeted Customer Income Bins DAX formula</t>
-  </si>
-  <si>
     <t>5 Predicted customer Income linear regression formula</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>4 Recommended Product Bins DAX formula</t>
   </si>
 </sst>
 </file>
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD328A0-A231-4F37-9A45-D654683D7BC9}">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +841,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -884,7 +884,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -907,7 +907,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -930,7 +930,7 @@
         <v>27</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -953,7 +953,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1000,7 +1000,7 @@
         <v>37</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>38</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1018,7 +1018,7 @@
         <v>39</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,7 @@
         <v>41</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,7 @@
         <v>42</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>43</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1062,7 +1062,7 @@
         <v>44</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1071,7 +1071,7 @@
         <v>45</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>46</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1089,7 +1089,7 @@
         <v>47</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1098,7 +1098,7 @@
         <v>48</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1113,33 +1113,33 @@
         <v>49</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="43.5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="52.5" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="B53" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="29.25" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="B55" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
@@ -1147,7 +1147,7 @@
         <v>53</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
@@ -1155,7 +1155,7 @@
         <v>54</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -1191,7 +1191,7 @@
         <v>60</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -1199,7 +1199,7 @@
         <v>61</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -1235,7 +1235,7 @@
         <v>67</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -1243,7 +1243,7 @@
         <v>68</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -1251,7 +1251,7 @@
         <v>69</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -1259,7 +1259,7 @@
         <v>70</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -1267,7 +1267,7 @@
         <v>71</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>